<commit_message>
Invalid Login Test was added. Twitter language selection was implemented
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Users/Users.xlsx
+++ b/src/test/resources/TestData/Users/Users.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Username</t>
   </si>
@@ -39,6 +39,12 @@
   </si>
   <si>
     <t>bkxEGLmduZeG4UaiSLQn</t>
+  </si>
+  <si>
+    <t>InvalidUser</t>
+  </si>
+  <si>
+    <t>InvalidPassword</t>
   </si>
 </sst>
 </file>
@@ -357,7 +363,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
@@ -393,6 +399,18 @@
         <v>1</v>
       </c>
     </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Simple TestNG management file was added. Publish & Delete tweet tests were implemented
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Users/Users.xlsx
+++ b/src/test/resources/TestData/Users/Users.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Username</t>
   </si>
@@ -41,10 +41,13 @@
     <t>bkxEGLmduZeG4UaiSLQn</t>
   </si>
   <si>
-    <t>InvalidUser</t>
-  </si>
-  <si>
     <t>InvalidPassword</t>
+  </si>
+  <si>
+    <t>Id</t>
+  </si>
+  <si>
+    <t>InvalidUserName</t>
   </si>
 </sst>
 </file>
@@ -363,50 +366,60 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" t="b">
+      <c r="D2" t="b">
         <f>TRUE</f>
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
         <v>5</v>
       </c>
-      <c r="B3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" t="b">
+      <c r="D3" t="b">
         <f>FALSE</f>
         <v>0</v>
       </c>

</xml_diff>